<commit_message>
Admin: Functional testing completed
</commit_message>
<xml_diff>
--- a/functional-testing-theCocktailShaker.xlsx
+++ b/functional-testing-theCocktailShaker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ae6e5f45dd1637aa/Pictures/theCocktailShaker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="150" documentId="8_{B860DF56-41DD-4CDE-93D8-8D16511ADA5D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3B7E927E-426A-4D1F-A2FE-2A0DB2D4E981}"/>
+  <xr:revisionPtr revIDLastSave="279" documentId="8_{B860DF56-41DD-4CDE-93D8-8D16511ADA5D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{10024F44-E22F-4328-ADC6-369FD666BB71}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{03B9E1AB-B057-4131-934D-AE2E63AFD17C}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="48">
   <si>
     <t>Pass</t>
   </si>
@@ -59,27 +59,9 @@
     <t>Clicking in the "First Ingredient" text input renders an ingredient list</t>
   </si>
   <si>
-    <t>Typing in the "First Ingredient" text input filters the ingredient list</t>
-  </si>
-  <si>
-    <t>Clicking on an ingredient in the "First Ingredient" ingredient list adds it to the text input box</t>
-  </si>
-  <si>
     <t>Clicking in the "Second Ingredient" text input renders an ingredient list</t>
   </si>
   <si>
-    <t>Typing in the "Second Ingredient" text input filters the ingredient list</t>
-  </si>
-  <si>
-    <t>Clicking on an ingredient in the "Second Ingredient" ingredient list adds it to the text input box</t>
-  </si>
-  <si>
-    <t>Clicking the "Shake it for me!" button when both text boxes are empty does not search</t>
-  </si>
-  <si>
-    <t>Clicking the "Shake it for me!" when a text box contains a spelling mistake does not search</t>
-  </si>
-  <si>
     <t>The previous cocktail button is disabled when the first available cocktail shows</t>
   </si>
   <si>
@@ -144,6 +126,57 @@
   </si>
   <si>
     <t>The "I fancy another go" button links to index.html</t>
+  </si>
+  <si>
+    <t>Typing in the "Second Ingredient" text input filters the second ingredient list</t>
+  </si>
+  <si>
+    <t>Typing in the "First Ingredient" text input filters the first ingredient list</t>
+  </si>
+  <si>
+    <t>Clicking the "Shake it for me!" when the first ingredient is mispelt and the second ingredient is correct or blank displays the correct error</t>
+  </si>
+  <si>
+    <t>Clicking the "Shake it for me!" button when the first input is blank displays the correct error</t>
+  </si>
+  <si>
+    <t>Clicking the "Shake it for me!" when both ingredients are mispelt displays the correct error</t>
+  </si>
+  <si>
+    <t>Clicking the "Shake it for me!" when the first ingredient is valid and the second ingredient is blank completes a search</t>
+  </si>
+  <si>
+    <t>Clicking the "Shake it for me!" when the first ingredient is valid and the second ingredient is mispelt displays the correct error</t>
+  </si>
+  <si>
+    <t>Clicking the "Shake it for me!" when both ingredients are valid completes a rearch</t>
+  </si>
+  <si>
+    <t>Clicking the "Shake it for me!" when both ingredients are the same</t>
+  </si>
+  <si>
+    <t>Typing an ingredient with different capitalisation does not result in an error i.e. GiN still works</t>
+  </si>
+  <si>
+    <t>Coconut Cream is an ingredient that doesn't return a cocktail - when used alone is the first ingredient it advises as such</t>
+  </si>
+  <si>
+    <t>Clicking on an ingredient in the "First Ingredient" ingredient list adds it to the first text input box</t>
+  </si>
+  <si>
+    <t>Clicking on an ingredient in the "Second Ingredient" ingredient list adds it to the second text input box</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>Coconut Cream is an ingredient that doesn't return a cocktail - as the first ingredient of two you should be advised that there are no cocktails</t>
+  </si>
+  <si>
+    <t>When you re-search with just coconut cream you should be advised that there are no cocktails</t>
+  </si>
+  <si>
+    <t>Coconut Cream is an ingredient that doesn't return a cocktail - as the second ingredient of two you should be advised that there are no cocktails</t>
   </si>
 </sst>
 </file>
@@ -159,7 +192,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -190,8 +223,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -214,11 +253,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -229,23 +279,121 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -560,15 +708,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C53A87AE-CCFF-4881-BEAF-6D70C3416B6F}">
-  <dimension ref="A1:E59"/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="111" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="117.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="13.21875" style="1" customWidth="1"/>
     <col min="6" max="7" width="13.21875" customWidth="1"/>
     <col min="8" max="8" width="12.77734375" bestFit="1" customWidth="1"/>
@@ -587,16 +735,16 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="8"/>
+      <c r="A3" s="6"/>
       <c r="B3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="9"/>
+      <c r="B5" s="8"/>
       <c r="C5"/>
       <c r="D5"/>
       <c r="E5"/>
@@ -605,16 +753,20 @@
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="7"/>
+      <c r="B6" s="9" t="s">
+        <v>44</v>
+      </c>
       <c r="C6"/>
       <c r="D6"/>
       <c r="E6"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="7"/>
+      <c r="B7" s="9" t="s">
+        <v>44</v>
+      </c>
       <c r="C7"/>
       <c r="D7"/>
       <c r="E7"/>
@@ -623,322 +775,514 @@
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="7"/>
+      <c r="B8" s="9" t="s">
+        <v>44</v>
+      </c>
       <c r="C8"/>
       <c r="D8"/>
       <c r="E8"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
-      <c r="B9" s="6"/>
+      <c r="B9" s="9"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="9"/>
+      <c r="A10" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="8"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="7"/>
+      <c r="B11" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="7"/>
+        <v>7</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="7"/>
+        <v>32</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="7"/>
+        <v>42</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" s="7"/>
+        <v>31</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="7"/>
+        <v>43</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="7"/>
+        <v>34</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="7"/>
+        <v>33</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="11"/>
+        <v>35</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21" s="7"/>
+        <v>36</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" s="7"/>
+        <v>37</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B23" s="7"/>
+        <v>39</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B24" s="7"/>
+        <v>38</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B25" s="7"/>
+        <v>40</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B26" s="7"/>
+        <v>9</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B27" s="7"/>
+        <v>10</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B28" s="7"/>
+        <v>12</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B29" s="7"/>
+        <v>13</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B30" s="7"/>
+        <v>14</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B31" s="7"/>
+        <v>16</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B32" s="7"/>
+        <v>17</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B33" s="7"/>
+        <v>18</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="7"/>
+      <c r="B34" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B35" s="7"/>
+        <v>19</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B36" s="7"/>
+        <v>27</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B37" s="9"/>
+      <c r="A37" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B38" s="7"/>
+        <v>21</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B39" s="7"/>
+        <v>20</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B40" s="7"/>
+        <v>22</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B41" s="7"/>
+        <v>23</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B42" s="7"/>
+        <v>41</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B43" s="7"/>
+        <v>45</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B44" s="7"/>
+      <c r="A44" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B45" s="7"/>
+        <v>47</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="5" t="s">
+      <c r="A46" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B46" s="7"/>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B47" s="7"/>
+      <c r="B47" s="8"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B48" s="7"/>
+        <v>5</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B49" s="7"/>
+        <v>9</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B50" s="7"/>
+        <v>10</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B51" s="7"/>
+        <v>12</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B52" s="7"/>
+        <v>13</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B53" s="7"/>
+        <v>14</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B54" s="7"/>
+        <v>16</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B55" s="9"/>
+      <c r="A55" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B56" s="7"/>
+        <v>18</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B57" s="7"/>
+        <v>26</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B58" s="7"/>
+        <v>19</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B59" s="7"/>
+        <v>27</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B62" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B64" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B65" s="8"/>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B66" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B67" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B69" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A65:B65"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A47:B47"/>
   </mergeCells>
+  <conditionalFormatting sqref="B6:B9">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="n">
+      <formula>NOT(ISERROR(SEARCH("n",B6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="y">
+      <formula>NOT(ISERROR(SEARCH("y",B6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B11:B46 B48:B64 B66:B69">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="n">
+      <formula>NOT(ISERROR(SEARCH("n",B11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="y">
+      <formula>NOT(ISERROR(SEARCH("y",B11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Admin: Final functional test completed
</commit_message>
<xml_diff>
--- a/functional-testing-theCocktailShaker.xlsx
+++ b/functional-testing-theCocktailShaker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ae6e5f45dd1637aa/Pictures/theCocktailShaker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="279" documentId="8_{B860DF56-41DD-4CDE-93D8-8D16511ADA5D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{10024F44-E22F-4328-ADC6-369FD666BB71}"/>
+  <xr:revisionPtr revIDLastSave="350" documentId="8_{B860DF56-41DD-4CDE-93D8-8D16511ADA5D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C25231D5-2D56-4C9B-806C-E5E981718448}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{03B9E1AB-B057-4131-934D-AE2E63AFD17C}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="49">
   <si>
     <t>Pass</t>
   </si>
@@ -119,9 +119,6 @@
     <t>When the instructions are displayed the cocktail name, measures &amp; ingredients and instructions are displayed</t>
   </si>
   <si>
-    <t>Entering a valid syntax email address and clicking sent send an email</t>
-  </si>
-  <si>
     <t>Text with the heading "Enjoy!" is now displayed</t>
   </si>
   <si>
@@ -152,9 +149,6 @@
     <t>Clicking the "Shake it for me!" when both ingredients are valid completes a rearch</t>
   </si>
   <si>
-    <t>Clicking the "Shake it for me!" when both ingredients are the same</t>
-  </si>
-  <si>
     <t>Typing an ingredient with different capitalisation does not result in an error i.e. GiN still works</t>
   </si>
   <si>
@@ -177,6 +171,15 @@
   </si>
   <si>
     <t>Coconut Cream is an ingredient that doesn't return a cocktail - as the second ingredient of two you should be advised that there are no cocktails</t>
+  </si>
+  <si>
+    <t>Clicking the "Shake it for me!" when both ingredients are the same displays the correct error</t>
+  </si>
+  <si>
+    <t>Entering an invalid syntax email address and clicking send displays an error message</t>
+  </si>
+  <si>
+    <t>Entering a valid syntax email address and clicking send, sends an email</t>
   </si>
 </sst>
 </file>
@@ -281,18 +284,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -330,66 +333,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -708,10 +651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C53A87AE-CCFF-4881-BEAF-6D70C3416B6F}">
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -741,10 +684,10 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="8"/>
+      <c r="B5" s="10"/>
       <c r="C5"/>
       <c r="D5"/>
       <c r="E5"/>
@@ -753,8 +696,8 @@
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>44</v>
+      <c r="B6" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="C6"/>
       <c r="D6"/>
@@ -764,8 +707,8 @@
       <c r="A7" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>44</v>
+      <c r="B7" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="C7"/>
       <c r="D7"/>
@@ -775,8 +718,8 @@
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>44</v>
+      <c r="B8" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="C8"/>
       <c r="D8"/>
@@ -784,481 +727,487 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
-      <c r="B9" s="9"/>
+      <c r="B9" s="8"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="8"/>
+      <c r="B10" s="10"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>44</v>
+      <c r="B11" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>44</v>
+      <c r="B12" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>44</v>
+        <v>31</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>44</v>
+        <v>40</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="9" t="s">
-        <v>44</v>
+      <c r="B15" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>44</v>
+        <v>30</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>44</v>
+        <v>41</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>44</v>
+        <v>33</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>44</v>
+        <v>32</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>44</v>
+        <v>34</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>44</v>
+        <v>35</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>44</v>
+        <v>36</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>44</v>
+        <v>46</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>44</v>
+        <v>37</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>44</v>
+        <v>38</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="9" t="s">
-        <v>44</v>
+      <c r="B26" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="9" t="s">
-        <v>44</v>
+      <c r="B27" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="9" t="s">
-        <v>44</v>
+      <c r="B28" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B29" s="9" t="s">
-        <v>44</v>
+      <c r="B29" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B30" s="9" t="s">
-        <v>44</v>
+      <c r="B30" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B31" s="9" t="s">
-        <v>44</v>
+      <c r="B31" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B32" s="9" t="s">
-        <v>44</v>
+      <c r="B32" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B33" s="9" t="s">
-        <v>44</v>
+      <c r="B33" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="9" t="s">
-        <v>44</v>
+      <c r="B34" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B35" s="9" t="s">
-        <v>44</v>
+      <c r="B35" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B36" s="9" t="s">
-        <v>44</v>
+      <c r="B36" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B37" s="9" t="s">
-        <v>44</v>
+      <c r="B37" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B38" s="9" t="s">
-        <v>44</v>
+      <c r="B38" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B39" s="9" t="s">
-        <v>44</v>
+      <c r="B39" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B40" s="9" t="s">
-        <v>44</v>
+      <c r="B40" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B41" s="9" t="s">
-        <v>44</v>
+      <c r="B41" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>44</v>
+        <v>39</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B43" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="9" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>44</v>
+      <c r="B44" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B45" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="9" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B46" s="9" t="s">
-        <v>44</v>
+      <c r="B46" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="8" t="s">
+      <c r="A47" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B47" s="8"/>
+      <c r="B47" s="10"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B48" s="9" t="s">
-        <v>44</v>
+      <c r="B48" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B49" s="9" t="s">
-        <v>44</v>
+      <c r="B49" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B50" s="9" t="s">
-        <v>44</v>
+      <c r="B50" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B51" s="9" t="s">
-        <v>44</v>
+      <c r="B51" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B52" s="9" t="s">
-        <v>44</v>
+      <c r="B52" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B53" s="9" t="s">
-        <v>44</v>
+      <c r="B53" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B54" s="9" t="s">
-        <v>44</v>
+      <c r="B54" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B55" s="9" t="s">
-        <v>44</v>
+      <c r="B55" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B56" s="9" t="s">
-        <v>44</v>
+      <c r="B56" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B57" s="9" t="s">
-        <v>44</v>
+      <c r="B57" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B58" s="9" t="s">
-        <v>44</v>
+      <c r="B58" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B59" s="9" t="s">
-        <v>44</v>
+      <c r="B59" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B60" s="9" t="s">
-        <v>44</v>
+      <c r="B60" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B61" s="9" t="s">
-        <v>44</v>
+      <c r="B61" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B62" s="9" t="s">
-        <v>44</v>
+      <c r="B62" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B63" s="9" t="s">
-        <v>44</v>
+      <c r="B63" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B64" s="9" t="s">
-        <v>44</v>
+      <c r="B64" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" s="8" t="s">
+      <c r="A65" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B65" s="8"/>
+      <c r="B65" s="10"/>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B66" s="9" t="s">
-        <v>44</v>
+      <c r="B66" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B67" s="9" t="s">
-        <v>44</v>
+        <v>47</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B68" s="9" t="s">
-        <v>44</v>
+        <v>48</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B69" s="9" t="s">
-        <v>44</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B70" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1275,7 +1224,7 @@
       <formula>NOT(ISERROR(SEARCH("y",B6)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B11:B46 B48:B64 B66:B69">
+  <conditionalFormatting sqref="B11:B46 B48:B64 B66:B70">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="n">
       <formula>NOT(ISERROR(SEARCH("n",B11)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
Admin: README wording changes
</commit_message>
<xml_diff>
--- a/functional-testing-theCocktailShaker.xlsx
+++ b/functional-testing-theCocktailShaker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ae6e5f45dd1637aa/Pictures/theCocktailShaker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="350" documentId="8_{B860DF56-41DD-4CDE-93D8-8D16511ADA5D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C25231D5-2D56-4C9B-806C-E5E981718448}"/>
+  <xr:revisionPtr revIDLastSave="351" documentId="8_{B860DF56-41DD-4CDE-93D8-8D16511ADA5D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3FC6EFFC-3F37-490D-9B7B-1875D109F08C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{03B9E1AB-B057-4131-934D-AE2E63AFD17C}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="49">
   <si>
     <t>Pass</t>
   </si>
@@ -653,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C53A87AE-CCFF-4881-BEAF-6D70C3416B6F}">
   <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1207,7 +1207,9 @@
       <c r="A70" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B70" s="8"/>
+      <c r="B70" s="8" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Admin: Updated functional testing
</commit_message>
<xml_diff>
--- a/functional-testing-theCocktailShaker.xlsx
+++ b/functional-testing-theCocktailShaker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ae6e5f45dd1637aa/Pictures/theCocktailShaker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="351" documentId="8_{B860DF56-41DD-4CDE-93D8-8D16511ADA5D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3FC6EFFC-3F37-490D-9B7B-1875D109F08C}"/>
+  <xr:revisionPtr revIDLastSave="418" documentId="8_{B860DF56-41DD-4CDE-93D8-8D16511ADA5D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{ED34DA08-EB44-4833-B2E5-2607D1DD4FBA}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{03B9E1AB-B057-4131-934D-AE2E63AFD17C}"/>
   </bookViews>
@@ -101,9 +101,6 @@
     <t>When "We've got to the end of that little selection" is displayed both the previous and home buttons are enabled</t>
   </si>
   <si>
-    <t>When "We've got to the end of that little selection" is displayed the "Show me a random selection" button links to ransom.html</t>
-  </si>
-  <si>
     <t>When "We've got to the end of that little selection" is displayed the "Let me choose ingredients" button displays the ingredient inputs</t>
   </si>
   <si>
@@ -180,6 +177,9 @@
   </si>
   <si>
     <t>Entering a valid syntax email address and clicking send, sends an email</t>
+  </si>
+  <si>
+    <t>When "We've got to the end of that little selection" is displayed the "Show me a random selection" button links to random.html</t>
   </si>
 </sst>
 </file>
@@ -653,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C53A87AE-CCFF-4881-BEAF-6D70C3416B6F}">
   <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -697,7 +697,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6"/>
       <c r="D6"/>
@@ -708,7 +708,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7"/>
       <c r="D7"/>
@@ -719,7 +719,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8"/>
       <c r="D8"/>
@@ -740,7 +740,7 @@
         <v>5</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -748,23 +748,23 @@
         <v>7</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -772,87 +772,87 @@
         <v>8</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -860,7 +860,7 @@
         <v>9</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -868,7 +868,7 @@
         <v>10</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -876,7 +876,7 @@
         <v>12</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -884,7 +884,7 @@
         <v>13</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -892,7 +892,7 @@
         <v>14</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -900,7 +900,7 @@
         <v>16</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -908,7 +908,7 @@
         <v>17</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -916,15 +916,15 @@
         <v>18</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -932,15 +932,15 @@
         <v>19</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -948,7 +948,7 @@
         <v>15</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -956,7 +956,7 @@
         <v>21</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -964,68 +964,68 @@
         <v>20</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B47" s="10"/>
     </row>
@@ -1034,7 +1034,7 @@
         <v>5</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
@@ -1042,7 +1042,7 @@
         <v>9</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
@@ -1050,7 +1050,7 @@
         <v>10</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
@@ -1058,7 +1058,7 @@
         <v>12</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
@@ -1066,7 +1066,7 @@
         <v>13</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
@@ -1074,7 +1074,7 @@
         <v>14</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
@@ -1082,7 +1082,7 @@
         <v>16</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
@@ -1090,7 +1090,7 @@
         <v>17</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
@@ -1098,15 +1098,15 @@
         <v>18</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
@@ -1114,15 +1114,15 @@
         <v>19</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
@@ -1130,7 +1130,7 @@
         <v>15</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
@@ -1138,7 +1138,7 @@
         <v>21</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
@@ -1146,28 +1146,28 @@
         <v>20</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B65" s="10"/>
     </row>
@@ -1176,39 +1176,39 @@
         <v>5</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>